<commit_message>
Updated firewall rules for VLAN table
</commit_message>
<xml_diff>
--- a/docs/vlan table.xlsx
+++ b/docs/vlan table.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\c99ma\Documents\School Fall 25\sys admin\group proj\IT-C-344---System-Administration-Project\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micke\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BF16248-5B49-41FE-AAA7-92D9BCCD5C84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8FC834F-77A9-487A-B481-733643EC9AE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21705" yWindow="-13470" windowWidth="21810" windowHeight="19305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -69,13 +69,28 @@
     <t>Employee Workstations</t>
   </si>
   <si>
-    <t>Allow Workstations → DNS TCP/UDP 53, Allow Workstations → Web TCP 80/443, Deny inter-VLAN traffic</t>
-  </si>
-  <si>
-    <t>Allow Management VLAN → all servers (necessary ports only), Deny all other access</t>
-  </si>
-  <si>
-    <t>Allow WAN → Web Server TCP 443/80, Allow Management VLAN → Web Server TCP 22/3389, Deny all else, Allow Web Servers → Database TCP 3306, Allow Management VLAN → Database TCP 3306, Deny all else, Allow Management VLAN → File Server TCP 445/139, Allow Workstations VLAN → File Server TCP 445/139, Allow Management VLAN → SIEM TCP 514/443, Allow SIEM → all servers for log collection, Deny all else, Allow Management VLAN → Backup TCP 22/873/445, Deny all else, Allow Admin VLAN → all servers (necessary ports only), Allow Admin → VPN TCP 1194, Deny all else</t>
+    <t xml:space="preserve">
+Allow WAN → Web Server TCP 443/80, 
+Allow Management VLAN → Web Server TCP 22/3389, 
+Deny all else, 
+Allow Web Servers → Database TCP 3306, 
+Allow VLAN 201 → Database TCP 3306, 
+Deny all else, 
+Allow VLAN 201 → File Server TCP 445/139,
+Allow VLAN 202 → File Server TCP 445/139, 
+Allow VLAN 201 → SIEM TCP 514/443, 
+Allow SIEM → all servers for log collection, 
+Deny all else, 
+Allow VLAN 201 → Backup TCP 22/873/445, 
+Deny all else, 
+Allow VLAN 201 → all servers (necessary ports only), 
+Allow Admin → VPN TCP 1194, Deny all else</t>
+  </si>
+  <si>
+    <t>Allow VLAN 201 → all servers (necessary ports only), Deny all other access</t>
+  </si>
+  <si>
+    <t>Allow VLAN 202 → DNS TCP/UDP 53, Allow VLAN 202 → Web TCP 80/443, Deny inter-VLAN traffic</t>
   </si>
 </sst>
 </file>
@@ -429,22 +444,22 @@
   <dimension ref="E2:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="8.88671875" style="2"/>
-    <col min="5" max="5" width="8.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.33203125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="33.33203125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="38.44140625" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="4" width="8.85546875" style="2"/>
+    <col min="5" max="5" width="8.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="33.28515625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="38.42578125" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="5:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="5:9" ht="30.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="5:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E3" s="1" t="s">
         <v>0</v>
       </c>
@@ -461,7 +476,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="5:9" ht="63.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="5:9" ht="63.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E4" s="2">
         <v>200</v>
       </c>
@@ -475,10 +490,10 @@
         <v>11</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="5" spans="5:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="5:9" ht="30" x14ac:dyDescent="0.25">
       <c r="E5" s="2">
         <v>201</v>
       </c>
@@ -495,7 +510,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="5:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="5:9" ht="45" x14ac:dyDescent="0.25">
       <c r="E6" s="2">
         <v>202</v>
       </c>
@@ -509,7 +524,7 @@
         <v>13</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>